<commit_message>
funciones concatenarmax y copiarnombre
</commit_message>
<xml_diff>
--- a/Alternadores-MercadoLibre.xlsx
+++ b/Alternadores-MercadoLibre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Desktop\Lekar-Automotriz\George\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Desktop\Lekar-Automotriz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E14306E-2F90-432D-90D5-960F35DD2C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA64D6B-14A1-4843-9B65-24A86A6009E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2940" yWindow="2940" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ayuda" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10605" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10303" uniqueCount="1015">
   <si>
     <t>Publica varios productos a la vez</t>
   </si>
@@ -5170,111 +5170,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="61" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -5292,11 +5187,116 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -5347,30 +5347,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FFA61C00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCFCFCF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCFCFCF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCFCFCF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCFCFCF"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FFA61C00"/>
@@ -5533,6 +5509,30 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCFCFCF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCFCFCF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCFCFCF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCFCFCF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA61C00"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
       <border>
@@ -8063,21 +8063,21 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
+      <c r="A4" s="167"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="168"/>
+      <c r="M4" s="168"/>
+      <c r="N4" s="168"/>
+      <c r="O4" s="168"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -8091,21 +8091,21 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
+      <c r="A5" s="169"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
+      <c r="K5" s="155"/>
+      <c r="L5" s="155"/>
+      <c r="M5" s="155"/>
+      <c r="N5" s="155"/>
+      <c r="O5" s="155"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -8119,21 +8119,21 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="93"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
+      <c r="A6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="171"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="177"/>
+      <c r="L6" s="177"/>
+      <c r="M6" s="177"/>
+      <c r="N6" s="177"/>
+      <c r="O6" s="177"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -8153,8 +8153,8 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="100"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="174"/>
       <c r="G7" s="19" t="s">
         <v>3</v>
       </c>
@@ -8180,11 +8180,11 @@
     </row>
     <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="100"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="174"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
       <c r="I8" s="25"/>
@@ -8208,23 +8208,23 @@
     </row>
     <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="168" t="s">
+      <c r="B9" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="169"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="100"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="174"/>
       <c r="G9" s="24"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="171" t="s">
+      <c r="I9" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="172"/>
-      <c r="K9" s="172"/>
-      <c r="L9" s="172"/>
-      <c r="M9" s="172"/>
-      <c r="N9" s="173"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="94"/>
       <c r="O9" s="28"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -8240,22 +8240,22 @@
     </row>
     <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="174"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="100"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="174"/>
       <c r="G10" s="24"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="175" t="str">
+      <c r="I10" s="96" t="str">
         <f>HYPERLINK("https://www.mercadolibre.com.co/publicar-masivamente/upload","subir la planilla excel")</f>
         <v>subir la planilla excel</v>
       </c>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="129"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="98"/>
       <c r="O10" s="28"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -8271,21 +8271,21 @@
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="158"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="97"/>
-      <c r="F11" s="100"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="174"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="176" t="s">
+      <c r="I11" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="177"/>
-      <c r="K11" s="177"/>
-      <c r="L11" s="177"/>
-      <c r="M11" s="177"/>
-      <c r="N11" s="178"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="104"/>
       <c r="O11" s="26"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -8301,11 +8301,11 @@
     </row>
     <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
-      <c r="B12" s="158"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="100"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="165"/>
+      <c r="F12" s="174"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="31"/>
@@ -8329,21 +8329,21 @@
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
-      <c r="B13" s="158"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="165" t="s">
+      <c r="B13" s="99"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="166"/>
-      <c r="I13" s="166"/>
-      <c r="J13" s="166"/>
-      <c r="K13" s="166"/>
-      <c r="L13" s="166"/>
-      <c r="M13" s="166"/>
-      <c r="N13" s="167"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="107"/>
       <c r="O13" s="26"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -8359,19 +8359,19 @@
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
-      <c r="B14" s="158"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="155"/>
-      <c r="H14" s="156"/>
-      <c r="I14" s="156"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="156"/>
-      <c r="M14" s="156"/>
-      <c r="N14" s="157"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="174"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="110"/>
       <c r="O14" s="26"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -8390,8 +8390,8 @@
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="100"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="174"/>
       <c r="G15" s="32" t="s">
         <v>6</v>
       </c>
@@ -8420,8 +8420,8 @@
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="100"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="174"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
       <c r="I16" s="33"/>
@@ -8448,18 +8448,18 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="152"/>
-      <c r="H17" s="153"/>
-      <c r="I17" s="154" t="s">
+      <c r="E17" s="165"/>
+      <c r="F17" s="174"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="116"/>
+      <c r="I17" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="143"/>
-      <c r="K17" s="143"/>
-      <c r="L17" s="143"/>
-      <c r="M17" s="143"/>
-      <c r="N17" s="117"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="119"/>
       <c r="O17" s="26"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -8478,16 +8478,16 @@
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="100"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="174"/>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="117"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="119"/>
       <c r="O18" s="26"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -8506,16 +8506,16 @@
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="100"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="174"/>
       <c r="G19" s="33"/>
       <c r="H19" s="33"/>
-      <c r="I19" s="138"/>
-      <c r="J19" s="138"/>
-      <c r="K19" s="138"/>
-      <c r="L19" s="138"/>
-      <c r="M19" s="138"/>
-      <c r="N19" s="139"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
+      <c r="N19" s="114"/>
       <c r="O19" s="26"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -8534,16 +8534,16 @@
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="160"/>
-      <c r="I20" s="160"/>
-      <c r="J20" s="160"/>
-      <c r="K20" s="160"/>
-      <c r="L20" s="160"/>
-      <c r="M20" s="160"/>
-      <c r="N20" s="161"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="174"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="121"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="121"/>
+      <c r="M20" s="121"/>
+      <c r="N20" s="122"/>
       <c r="O20" s="26"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -8562,8 +8562,8 @@
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="100"/>
+      <c r="E21" s="165"/>
+      <c r="F21" s="174"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
@@ -8587,11 +8587,11 @@
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="100"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="165"/>
+      <c r="F22" s="174"/>
       <c r="G22" s="35" t="s">
         <v>8</v>
       </c>
@@ -8620,16 +8620,16 @@
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="155"/>
-      <c r="H23" s="156"/>
-      <c r="I23" s="156"/>
-      <c r="J23" s="156"/>
-      <c r="K23" s="156"/>
-      <c r="L23" s="156"/>
-      <c r="M23" s="156"/>
-      <c r="N23" s="157"/>
+      <c r="E23" s="165"/>
+      <c r="F23" s="174"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="109"/>
+      <c r="N23" s="110"/>
       <c r="O23" s="40"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -8645,22 +8645,22 @@
     </row>
     <row r="24" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
-      <c r="B24" s="158"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="162" t="s">
+      <c r="B24" s="99"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="165"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="163"/>
-      <c r="I24" s="163"/>
-      <c r="J24" s="163"/>
-      <c r="K24" s="163"/>
-      <c r="L24" s="163"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="163"/>
-      <c r="O24" s="163"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="124"/>
+      <c r="K24" s="124"/>
+      <c r="L24" s="124"/>
+      <c r="M24" s="124"/>
+      <c r="N24" s="124"/>
+      <c r="O24" s="124"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
@@ -8675,20 +8675,20 @@
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="138"/>
-      <c r="I25" s="138"/>
-      <c r="J25" s="138"/>
-      <c r="K25" s="138"/>
-      <c r="L25" s="138"/>
-      <c r="M25" s="138"/>
-      <c r="N25" s="138"/>
-      <c r="O25" s="138"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="125"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="113"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -8703,21 +8703,21 @@
     </row>
     <row r="26" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
-      <c r="B26" s="140"/>
-      <c r="C26" s="141"/>
-      <c r="D26" s="142"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="100"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="131"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="174"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="135" t="s">
+      <c r="I26" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="136"/>
-      <c r="K26" s="136"/>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
-      <c r="N26" s="115"/>
+      <c r="J26" s="127"/>
+      <c r="K26" s="127"/>
+      <c r="L26" s="127"/>
+      <c r="M26" s="127"/>
+      <c r="N26" s="128"/>
       <c r="O26" s="39"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
@@ -8733,19 +8733,19 @@
     </row>
     <row r="27" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="41"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="145"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="100"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="174"/>
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="143"/>
-      <c r="K27" s="143"/>
-      <c r="L27" s="143"/>
-      <c r="M27" s="143"/>
-      <c r="N27" s="117"/>
+      <c r="I27" s="133"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="119"/>
       <c r="O27" s="26"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
@@ -8761,19 +8761,19 @@
     </row>
     <row r="28" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="41"/>
-      <c r="B28" s="144"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="100"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="165"/>
+      <c r="F28" s="174"/>
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
-      <c r="I28" s="116"/>
-      <c r="J28" s="143"/>
-      <c r="K28" s="143"/>
-      <c r="L28" s="143"/>
-      <c r="M28" s="143"/>
-      <c r="N28" s="117"/>
+      <c r="I28" s="133"/>
+      <c r="J28" s="118"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="118"/>
+      <c r="M28" s="118"/>
+      <c r="N28" s="119"/>
       <c r="O28" s="26"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -8789,19 +8789,19 @@
     </row>
     <row r="29" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43"/>
-      <c r="B29" s="144"/>
-      <c r="C29" s="145"/>
-      <c r="D29" s="146"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="100"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="165"/>
+      <c r="F29" s="174"/>
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
-      <c r="I29" s="116"/>
-      <c r="J29" s="143"/>
-      <c r="K29" s="143"/>
-      <c r="L29" s="143"/>
-      <c r="M29" s="143"/>
-      <c r="N29" s="117"/>
+      <c r="I29" s="133"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="118"/>
+      <c r="L29" s="118"/>
+      <c r="M29" s="118"/>
+      <c r="N29" s="119"/>
       <c r="O29" s="26"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
@@ -8817,19 +8817,19 @@
     </row>
     <row r="30" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43"/>
-      <c r="B30" s="144"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="147"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="100"/>
+      <c r="B30" s="134"/>
+      <c r="C30" s="135"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="174"/>
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="143"/>
-      <c r="K30" s="143"/>
-      <c r="L30" s="143"/>
-      <c r="M30" s="143"/>
-      <c r="N30" s="117"/>
+      <c r="I30" s="133"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="118"/>
+      <c r="N30" s="119"/>
       <c r="O30" s="26"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
@@ -8845,19 +8845,19 @@
     </row>
     <row r="31" spans="1:26" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43"/>
-      <c r="B31" s="144"/>
-      <c r="C31" s="145"/>
-      <c r="D31" s="147"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="100"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="135"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="165"/>
+      <c r="F31" s="174"/>
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="143"/>
-      <c r="K31" s="143"/>
-      <c r="L31" s="143"/>
-      <c r="M31" s="143"/>
-      <c r="N31" s="117"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="118"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
+      <c r="N31" s="119"/>
       <c r="O31" s="26"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
@@ -8873,22 +8873,22 @@
     </row>
     <row r="32" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44"/>
-      <c r="B32" s="144"/>
-      <c r="C32" s="145"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="100"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="165"/>
+      <c r="F32" s="174"/>
       <c r="G32" s="42"/>
       <c r="H32" s="42"/>
-      <c r="I32" s="127" t="str">
+      <c r="I32" s="138" t="str">
         <f>HYPERLINK("https://www.mercadolibre.com.co/ayuda/variantes-excel_5167","Quiero saber más")</f>
         <v>Quiero saber más</v>
       </c>
-      <c r="J32" s="128"/>
-      <c r="K32" s="128"/>
-      <c r="L32" s="128"/>
-      <c r="M32" s="128"/>
-      <c r="N32" s="129"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+      <c r="N32" s="98"/>
       <c r="O32" s="26"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
@@ -8904,19 +8904,19 @@
     </row>
     <row r="33" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="105"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="148"/>
-      <c r="H33" s="149"/>
-      <c r="I33" s="149"/>
-      <c r="J33" s="149"/>
-      <c r="K33" s="149"/>
-      <c r="L33" s="149"/>
-      <c r="M33" s="149"/>
-      <c r="N33" s="150"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="139"/>
+      <c r="H33" s="140"/>
+      <c r="I33" s="140"/>
+      <c r="J33" s="140"/>
+      <c r="K33" s="140"/>
+      <c r="L33" s="140"/>
+      <c r="M33" s="140"/>
+      <c r="N33" s="141"/>
       <c r="O33" s="26"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
@@ -8932,19 +8932,19 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="151"/>
-      <c r="H34" s="138"/>
-      <c r="I34" s="138"/>
-      <c r="J34" s="138"/>
-      <c r="K34" s="138"/>
-      <c r="L34" s="138"/>
-      <c r="M34" s="138"/>
-      <c r="N34" s="139"/>
+      <c r="B34" s="111"/>
+      <c r="C34" s="100"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="165"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="114"/>
       <c r="O34" s="26"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
@@ -8960,11 +8960,11 @@
     </row>
     <row r="35" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="106"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="100"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="101"/>
+      <c r="E35" s="165"/>
+      <c r="F35" s="174"/>
       <c r="G35" s="45" t="s">
         <v>11</v>
       </c>
@@ -8990,11 +8990,11 @@
     </row>
     <row r="36" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="105"/>
-      <c r="D36" s="106"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="100"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="100"/>
+      <c r="D36" s="101"/>
+      <c r="E36" s="165"/>
+      <c r="F36" s="174"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
@@ -9018,21 +9018,21 @@
     </row>
     <row r="37" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="106"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="100"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="165"/>
+      <c r="F37" s="174"/>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
-      <c r="I37" s="135" t="s">
+      <c r="I37" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="136"/>
-      <c r="K37" s="136"/>
-      <c r="L37" s="136"/>
-      <c r="M37" s="136"/>
-      <c r="N37" s="115"/>
+      <c r="J37" s="127"/>
+      <c r="K37" s="127"/>
+      <c r="L37" s="127"/>
+      <c r="M37" s="127"/>
+      <c r="N37" s="128"/>
       <c r="O37" s="46"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
@@ -9048,19 +9048,19 @@
     </row>
     <row r="38" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
-      <c r="B38" s="107"/>
-      <c r="C38" s="105"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="100"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="100"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="165"/>
+      <c r="F38" s="174"/>
       <c r="G38" s="24"/>
       <c r="H38" s="42"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="138"/>
-      <c r="K38" s="138"/>
-      <c r="L38" s="138"/>
-      <c r="M38" s="138"/>
-      <c r="N38" s="139"/>
+      <c r="I38" s="129"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="113"/>
+      <c r="N38" s="114"/>
       <c r="O38" s="46"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
@@ -9076,22 +9076,22 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
-      <c r="B39" s="107"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="100"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="100"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="165"/>
+      <c r="F39" s="174"/>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>
-      <c r="I39" s="127" t="str">
+      <c r="I39" s="138" t="str">
         <f>HYPERLINK("https://www.mercadolibre.com.co/ayuda/imagenesexcel_5121","Obtener las URLs de mis fotos")</f>
         <v>Obtener las URLs de mis fotos</v>
       </c>
-      <c r="J39" s="128"/>
-      <c r="K39" s="128"/>
-      <c r="L39" s="128"/>
-      <c r="M39" s="128"/>
-      <c r="N39" s="129"/>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="98"/>
       <c r="O39" s="23"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -9107,19 +9107,19 @@
     </row>
     <row r="40" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
-      <c r="B40" s="107"/>
-      <c r="C40" s="105"/>
-      <c r="D40" s="106"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="131"/>
-      <c r="I40" s="131"/>
-      <c r="J40" s="131"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="131"/>
-      <c r="M40" s="131"/>
-      <c r="N40" s="131"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="165"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="142"/>
+      <c r="H40" s="143"/>
+      <c r="I40" s="143"/>
+      <c r="J40" s="143"/>
+      <c r="K40" s="143"/>
+      <c r="L40" s="143"/>
+      <c r="M40" s="143"/>
+      <c r="N40" s="143"/>
       <c r="O40" s="26"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
@@ -9138,17 +9138,17 @@
       <c r="B41" s="47"/>
       <c r="C41" s="47"/>
       <c r="D41" s="47"/>
-      <c r="E41" s="97"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="132"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="133"/>
-      <c r="K41" s="133"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="133"/>
-      <c r="N41" s="133"/>
-      <c r="O41" s="134"/>
+      <c r="E41" s="165"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="144"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+      <c r="K41" s="145"/>
+      <c r="L41" s="145"/>
+      <c r="M41" s="145"/>
+      <c r="N41" s="145"/>
+      <c r="O41" s="146"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
@@ -9163,22 +9163,22 @@
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
-      <c r="B42" s="107"/>
-      <c r="C42" s="105"/>
-      <c r="D42" s="106"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="108" t="s">
+      <c r="B42" s="111"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="101"/>
+      <c r="E42" s="165"/>
+      <c r="F42" s="174"/>
+      <c r="G42" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="109"/>
-      <c r="I42" s="109"/>
-      <c r="J42" s="109"/>
-      <c r="K42" s="109"/>
-      <c r="L42" s="109"/>
-      <c r="M42" s="109"/>
-      <c r="N42" s="109"/>
-      <c r="O42" s="110"/>
+      <c r="H42" s="148"/>
+      <c r="I42" s="148"/>
+      <c r="J42" s="148"/>
+      <c r="K42" s="148"/>
+      <c r="L42" s="148"/>
+      <c r="M42" s="148"/>
+      <c r="N42" s="148"/>
+      <c r="O42" s="149"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
@@ -9193,20 +9193,20 @@
     </row>
     <row r="43" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
-      <c r="B43" s="107"/>
-      <c r="C43" s="105"/>
-      <c r="D43" s="106"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="111"/>
-      <c r="H43" s="112"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="112"/>
-      <c r="L43" s="112"/>
-      <c r="M43" s="112"/>
-      <c r="N43" s="112"/>
-      <c r="O43" s="113"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="100"/>
+      <c r="D43" s="101"/>
+      <c r="E43" s="166"/>
+      <c r="F43" s="174"/>
+      <c r="G43" s="150"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="151"/>
+      <c r="L43" s="151"/>
+      <c r="M43" s="151"/>
+      <c r="N43" s="151"/>
+      <c r="O43" s="152"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -9225,18 +9225,18 @@
       <c r="C44" s="47"/>
       <c r="D44" s="47"/>
       <c r="E44" s="48"/>
-      <c r="F44" s="100"/>
-      <c r="G44" s="114"/>
-      <c r="H44" s="115"/>
-      <c r="I44" s="118" t="s">
+      <c r="F44" s="174"/>
+      <c r="G44" s="153"/>
+      <c r="H44" s="128"/>
+      <c r="I44" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
-      <c r="M44" s="92"/>
-      <c r="N44" s="92"/>
-      <c r="O44" s="125"/>
+      <c r="J44" s="155"/>
+      <c r="K44" s="155"/>
+      <c r="L44" s="155"/>
+      <c r="M44" s="155"/>
+      <c r="N44" s="155"/>
+      <c r="O44" s="162"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -9251,20 +9251,20 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
-      <c r="B45" s="107"/>
-      <c r="C45" s="105"/>
-      <c r="D45" s="106"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="100"/>
-      <c r="G45" s="116"/>
-      <c r="H45" s="117"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="109"/>
-      <c r="K45" s="109"/>
-      <c r="L45" s="109"/>
-      <c r="M45" s="109"/>
-      <c r="N45" s="110"/>
-      <c r="O45" s="126"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="100"/>
+      <c r="D45" s="101"/>
+      <c r="E45" s="164"/>
+      <c r="F45" s="174"/>
+      <c r="G45" s="133"/>
+      <c r="H45" s="119"/>
+      <c r="I45" s="156"/>
+      <c r="J45" s="148"/>
+      <c r="K45" s="148"/>
+      <c r="L45" s="148"/>
+      <c r="M45" s="148"/>
+      <c r="N45" s="149"/>
+      <c r="O45" s="163"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -9279,23 +9279,23 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
-      <c r="B46" s="107"/>
-      <c r="C46" s="105"/>
-      <c r="D46" s="106"/>
-      <c r="E46" s="97"/>
-      <c r="F46" s="100"/>
-      <c r="G46" s="116"/>
-      <c r="H46" s="117"/>
-      <c r="I46" s="120" t="str">
+      <c r="B46" s="111"/>
+      <c r="C46" s="100"/>
+      <c r="D46" s="101"/>
+      <c r="E46" s="165"/>
+      <c r="F46" s="174"/>
+      <c r="G46" s="133"/>
+      <c r="H46" s="119"/>
+      <c r="I46" s="157" t="str">
         <f>HYPERLINK("https://www.mercadolibre.com.co/ayuda/805","¿Cómo sacar una buena foto para no perder exposición?")</f>
         <v>¿Cómo sacar una buena foto para no perder exposición?</v>
       </c>
-      <c r="J46" s="121"/>
-      <c r="K46" s="121"/>
-      <c r="L46" s="121"/>
-      <c r="M46" s="121"/>
-      <c r="N46" s="122"/>
-      <c r="O46" s="126"/>
+      <c r="J46" s="158"/>
+      <c r="K46" s="158"/>
+      <c r="L46" s="158"/>
+      <c r="M46" s="158"/>
+      <c r="N46" s="159"/>
+      <c r="O46" s="163"/>
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
@@ -9310,20 +9310,20 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
-      <c r="B47" s="107"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="106"/>
-      <c r="E47" s="97"/>
-      <c r="F47" s="100"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="117"/>
-      <c r="I47" s="123"/>
-      <c r="J47" s="92"/>
-      <c r="K47" s="92"/>
-      <c r="L47" s="92"/>
-      <c r="M47" s="92"/>
-      <c r="N47" s="124"/>
-      <c r="O47" s="126"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="100"/>
+      <c r="D47" s="101"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="174"/>
+      <c r="G47" s="133"/>
+      <c r="H47" s="119"/>
+      <c r="I47" s="160"/>
+      <c r="J47" s="155"/>
+      <c r="K47" s="155"/>
+      <c r="L47" s="155"/>
+      <c r="M47" s="155"/>
+      <c r="N47" s="161"/>
+      <c r="O47" s="163"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
@@ -9338,11 +9338,11 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
-      <c r="B48" s="107"/>
-      <c r="C48" s="105"/>
-      <c r="D48" s="106"/>
-      <c r="E48" s="97"/>
-      <c r="F48" s="100"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="101"/>
+      <c r="E48" s="165"/>
+      <c r="F48" s="174"/>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
       <c r="I48" s="49"/>
@@ -9366,11 +9366,11 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
-      <c r="B49" s="107"/>
-      <c r="C49" s="105"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="97"/>
-      <c r="F49" s="100"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="165"/>
+      <c r="F49" s="174"/>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
@@ -9394,11 +9394,11 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="107"/>
-      <c r="C50" s="105"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="97"/>
-      <c r="F50" s="100"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="100"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="165"/>
+      <c r="F50" s="174"/>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
       <c r="I50" s="49"/>
@@ -9422,11 +9422,11 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
-      <c r="B51" s="107"/>
-      <c r="C51" s="105"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="100"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="165"/>
+      <c r="F51" s="174"/>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
       <c r="I51" s="49"/>
@@ -9450,11 +9450,11 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
-      <c r="B52" s="107"/>
-      <c r="C52" s="105"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="100"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="165"/>
+      <c r="F52" s="174"/>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
       <c r="I52" s="49"/>
@@ -9478,11 +9478,11 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
-      <c r="B53" s="107"/>
-      <c r="C53" s="105"/>
-      <c r="D53" s="106"/>
-      <c r="E53" s="97"/>
-      <c r="F53" s="100"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="165"/>
+      <c r="F53" s="174"/>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
@@ -9506,11 +9506,11 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="105"/>
-      <c r="D54" s="106"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="100"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="100"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="165"/>
+      <c r="F54" s="174"/>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
@@ -9534,11 +9534,11 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
-      <c r="B55" s="107"/>
-      <c r="C55" s="105"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="100"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="165"/>
+      <c r="F55" s="174"/>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
       <c r="I55" s="49"/>
@@ -9562,11 +9562,11 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
-      <c r="B56" s="107"/>
-      <c r="C56" s="105"/>
-      <c r="D56" s="106"/>
-      <c r="E56" s="97"/>
-      <c r="F56" s="100"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="100"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="165"/>
+      <c r="F56" s="174"/>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
       <c r="I56" s="49"/>
@@ -9590,11 +9590,11 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
-      <c r="B57" s="107"/>
-      <c r="C57" s="105"/>
-      <c r="D57" s="106"/>
-      <c r="E57" s="97"/>
-      <c r="F57" s="100"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="100"/>
+      <c r="D57" s="101"/>
+      <c r="E57" s="165"/>
+      <c r="F57" s="174"/>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
@@ -9618,11 +9618,11 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
-      <c r="B58" s="107"/>
-      <c r="C58" s="105"/>
-      <c r="D58" s="106"/>
-      <c r="E58" s="97"/>
-      <c r="F58" s="100"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="100"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="165"/>
+      <c r="F58" s="174"/>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
       <c r="I58" s="49"/>
@@ -9646,11 +9646,11 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
-      <c r="B59" s="107"/>
-      <c r="C59" s="105"/>
-      <c r="D59" s="106"/>
-      <c r="E59" s="97"/>
-      <c r="F59" s="100"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="100"/>
+      <c r="D59" s="101"/>
+      <c r="E59" s="165"/>
+      <c r="F59" s="174"/>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
       <c r="I59" s="49"/>
@@ -9674,11 +9674,11 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
-      <c r="B60" s="107"/>
-      <c r="C60" s="105"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="97"/>
-      <c r="F60" s="100"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="100"/>
+      <c r="D60" s="101"/>
+      <c r="E60" s="165"/>
+      <c r="F60" s="174"/>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
       <c r="I60" s="49"/>
@@ -9702,11 +9702,11 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
-      <c r="B61" s="107"/>
-      <c r="C61" s="105"/>
-      <c r="D61" s="106"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="100"/>
+      <c r="B61" s="111"/>
+      <c r="C61" s="100"/>
+      <c r="D61" s="101"/>
+      <c r="E61" s="165"/>
+      <c r="F61" s="174"/>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
       <c r="I61" s="49"/>
@@ -9730,11 +9730,11 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
-      <c r="B62" s="107"/>
-      <c r="C62" s="105"/>
-      <c r="D62" s="106"/>
-      <c r="E62" s="97"/>
-      <c r="F62" s="100"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="101"/>
+      <c r="E62" s="165"/>
+      <c r="F62" s="174"/>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
       <c r="I62" s="49"/>
@@ -9758,11 +9758,11 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
-      <c r="B63" s="107"/>
-      <c r="C63" s="105"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="97"/>
-      <c r="F63" s="100"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="165"/>
+      <c r="F63" s="174"/>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
       <c r="I63" s="49"/>
@@ -9786,11 +9786,11 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
-      <c r="B64" s="107"/>
-      <c r="C64" s="105"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="97"/>
-      <c r="F64" s="100"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="101"/>
+      <c r="E64" s="165"/>
+      <c r="F64" s="174"/>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
       <c r="I64" s="49"/>
@@ -9814,11 +9814,11 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
-      <c r="B65" s="107"/>
-      <c r="C65" s="105"/>
-      <c r="D65" s="106"/>
-      <c r="E65" s="97"/>
-      <c r="F65" s="100"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="100"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="165"/>
+      <c r="F65" s="174"/>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
       <c r="I65" s="49"/>
@@ -9842,11 +9842,11 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
-      <c r="B66" s="107"/>
-      <c r="C66" s="105"/>
-      <c r="D66" s="106"/>
-      <c r="E66" s="97"/>
-      <c r="F66" s="100"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="100"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="165"/>
+      <c r="F66" s="174"/>
       <c r="G66" s="49"/>
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>
@@ -9870,11 +9870,11 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="105"/>
-      <c r="D67" s="106"/>
-      <c r="E67" s="97"/>
-      <c r="F67" s="100"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="100"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="165"/>
+      <c r="F67" s="174"/>
       <c r="G67" s="49"/>
       <c r="H67" s="49"/>
       <c r="I67" s="49"/>
@@ -9898,11 +9898,11 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
-      <c r="B68" s="107"/>
-      <c r="C68" s="105"/>
-      <c r="D68" s="106"/>
-      <c r="E68" s="97"/>
-      <c r="F68" s="100"/>
+      <c r="B68" s="111"/>
+      <c r="C68" s="100"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="165"/>
+      <c r="F68" s="174"/>
       <c r="G68" s="49"/>
       <c r="H68" s="49"/>
       <c r="I68" s="49"/>
@@ -9926,11 +9926,11 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
-      <c r="B69" s="107"/>
-      <c r="C69" s="105"/>
-      <c r="D69" s="106"/>
-      <c r="E69" s="97"/>
-      <c r="F69" s="100"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="100"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="165"/>
+      <c r="F69" s="174"/>
       <c r="G69" s="49"/>
       <c r="H69" s="49"/>
       <c r="I69" s="49"/>
@@ -9954,11 +9954,11 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
-      <c r="B70" s="107"/>
-      <c r="C70" s="105"/>
-      <c r="D70" s="106"/>
-      <c r="E70" s="98"/>
-      <c r="F70" s="101"/>
+      <c r="B70" s="111"/>
+      <c r="C70" s="100"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="166"/>
+      <c r="F70" s="175"/>
       <c r="G70" s="49"/>
       <c r="H70" s="49"/>
       <c r="I70" s="49"/>
@@ -15427,27 +15427,55 @@
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:N13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="G34:N34"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:N19"/>
-    <mergeCell ref="G23:N23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="G20:N20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="G24:O25"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:E43"/>
+    <mergeCell ref="F6:F70"/>
+    <mergeCell ref="G6:O6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="G42:O42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="G43:O43"/>
+    <mergeCell ref="G44:H47"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="I45:N45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="I47:N47"/>
+    <mergeCell ref="O44:O47"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E45:E70"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="G40:N40"/>
+    <mergeCell ref="G41:O41"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
@@ -15464,55 +15492,27 @@
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="G33:N33"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="I39:N39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="G40:N40"/>
-    <mergeCell ref="G41:O41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="G42:O42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="G43:O43"/>
-    <mergeCell ref="G44:H47"/>
-    <mergeCell ref="I44:N44"/>
-    <mergeCell ref="I45:N45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="I47:N47"/>
-    <mergeCell ref="O44:O47"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E45:E70"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A5:O5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:E43"/>
-    <mergeCell ref="F6:F70"/>
-    <mergeCell ref="G6:O6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="G34:N34"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:N19"/>
+    <mergeCell ref="G23:N23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="G20:N20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="G24:O25"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:N13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="I11:N11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" location="'Motores de Arranque'!A1" display="Motores de Arranque" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -15643,7 +15643,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -15676,61 +15676,61 @@
       <c r="A1" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="143"/>
+      <c r="B1" s="118"/>
       <c r="C1" s="186" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="143"/>
+      <c r="D1" s="118"/>
       <c r="E1" s="180"/>
       <c r="F1" s="188" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="143"/>
+      <c r="G1" s="118"/>
       <c r="H1" s="189"/>
       <c r="I1" s="190"/>
       <c r="J1" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
       <c r="O1" s="180"/>
-      <c r="P1" s="143"/>
+      <c r="P1" s="118"/>
       <c r="Q1" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="143"/>
+      <c r="R1" s="118"/>
       <c r="S1" s="180"/>
-      <c r="T1" s="143"/>
+      <c r="T1" s="118"/>
       <c r="U1" s="180"/>
-      <c r="V1" s="143"/>
+      <c r="V1" s="118"/>
     </row>
     <row r="2" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="183" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="118"/>
       <c r="C2" s="187"/>
-      <c r="D2" s="143"/>
+      <c r="D2" s="118"/>
       <c r="E2" s="180"/>
       <c r="F2" s="191"/>
-      <c r="G2" s="143"/>
+      <c r="G2" s="118"/>
       <c r="H2" s="189"/>
       <c r="I2" s="190"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
       <c r="O2" s="180"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="143"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
       <c r="S2" s="180"/>
-      <c r="T2" s="143"/>
+      <c r="T2" s="118"/>
       <c r="U2" s="180"/>
-      <c r="V2" s="143"/>
+      <c r="V2" s="118"/>
     </row>
     <row r="3" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
@@ -52104,37 +52104,37 @@
     <mergeCell ref="F1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:A1001">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>LEN(INDIRECT(ADDRESS(ROW(),COLUMN()))) &gt; 60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B1001">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>LEN(INDIRECT(ADDRESS(ROW() + (0),COLUMN() + (-1)))) &gt; 60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F1001">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>LEN(INDIRECT(ADDRESS(ROW(),COLUMN()))) &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F1001">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>LEN(INDIRECT(ADDRESS((ROW()),(1)))) &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G10001">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Nuevo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G1001">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>LEN(INDIRECT(ADDRESS(ROW(),COLUMN()))) &lt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J10001">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Clásica"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52144,42 +52144,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:L10001">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Seleccionar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:M10001">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"Seleccionar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N10001">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"Seleccionar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:O1001">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>ISTEXT(INDIRECT(ADDRESS(ROW(),COLUMN())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P10001">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>"Seleccionar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S1001">
-    <cfRule type="expression" dxfId="3" priority="14">
+    <cfRule type="expression" dxfId="2" priority="14">
       <formula>ISTEXT(INDIRECT(ADDRESS(ROW(),COLUMN())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6:T10001">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
       <formula>"Seleccionar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U1001">
-    <cfRule type="expression" dxfId="1" priority="16">
+    <cfRule type="expression" dxfId="0" priority="16">
       <formula>ISTEXT(INDIRECT(ADDRESS(ROW(),COLUMN())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52286,8 +52286,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AB305"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B303"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -76283,8 +76283,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:H599"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D303"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -76296,9 +76296,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="85"/>
       <c r="B2" s="85"/>
-      <c r="D2" s="86" t="s">
-        <v>107</v>
-      </c>
+      <c r="D2" s="86"/>
       <c r="E2" s="86"/>
       <c r="F2" s="86"/>
       <c r="G2" s="86"/>
@@ -76307,2109 +76305,1507 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
       <c r="B3" s="85"/>
-      <c r="D3" s="86" t="s">
-        <v>110</v>
-      </c>
+      <c r="D3" s="86"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="85"/>
       <c r="B4" s="85"/>
-      <c r="D4" s="86" t="s">
-        <v>114</v>
-      </c>
+      <c r="D4" s="86"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="85"/>
       <c r="B5" s="85"/>
-      <c r="D5" s="86" t="s">
-        <v>117</v>
-      </c>
+      <c r="D5" s="86"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="85"/>
       <c r="B6" s="85"/>
-      <c r="D6" s="86" t="s">
-        <v>121</v>
-      </c>
+      <c r="D6" s="86"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="85"/>
       <c r="B7" s="85"/>
-      <c r="D7" s="86" t="s">
-        <v>125</v>
-      </c>
+      <c r="D7" s="86"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
-      <c r="D8" s="86" t="s">
-        <v>129</v>
-      </c>
+      <c r="D8" s="86"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="85"/>
       <c r="B9" s="85"/>
-      <c r="D9" s="86" t="s">
-        <v>133</v>
-      </c>
+      <c r="D9" s="86"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="85"/>
       <c r="B10" s="85"/>
-      <c r="D10" s="86" t="s">
-        <v>137</v>
-      </c>
+      <c r="D10" s="86"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="85"/>
       <c r="B11" s="85"/>
-      <c r="D11" s="86" t="s">
-        <v>141</v>
-      </c>
+      <c r="D11" s="86"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="85"/>
       <c r="B12" s="85"/>
-      <c r="D12" s="86" t="s">
-        <v>145</v>
-      </c>
+      <c r="D12" s="86"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="85"/>
       <c r="B13" s="85"/>
-      <c r="D13" s="86" t="s">
-        <v>148</v>
-      </c>
+      <c r="D13" s="86"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="85"/>
       <c r="B14" s="85"/>
-      <c r="D14" s="86" t="s">
-        <v>151</v>
-      </c>
+      <c r="D14" s="86"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="85"/>
       <c r="B15" s="85"/>
-      <c r="D15" s="86" t="s">
-        <v>154</v>
-      </c>
+      <c r="D15" s="86"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="85"/>
       <c r="B16" s="85"/>
-      <c r="D16" s="86" t="s">
-        <v>157</v>
-      </c>
+      <c r="D16" s="86"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="85"/>
       <c r="B17" s="85"/>
-      <c r="D17" s="86" t="s">
-        <v>160</v>
-      </c>
+      <c r="D17" s="86"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="85"/>
       <c r="B18" s="85"/>
-      <c r="D18" s="86" t="s">
-        <v>163</v>
-      </c>
+      <c r="D18" s="86"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="85"/>
       <c r="B19" s="85"/>
-      <c r="D19" s="86" t="s">
-        <v>166</v>
-      </c>
+      <c r="D19" s="86"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="85"/>
       <c r="B20" s="85"/>
-      <c r="D20" s="86" t="s">
-        <v>169</v>
-      </c>
+      <c r="D20" s="86"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="85"/>
       <c r="B21" s="85"/>
-      <c r="D21" s="86" t="s">
-        <v>172</v>
-      </c>
+      <c r="D21" s="86"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="85"/>
       <c r="B22" s="85"/>
-      <c r="D22" s="86" t="s">
-        <v>176</v>
-      </c>
+      <c r="D22" s="86"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="85"/>
       <c r="B23" s="85"/>
-      <c r="D23" s="86" t="s">
-        <v>179</v>
-      </c>
+      <c r="D23" s="86"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="85"/>
       <c r="B24" s="85"/>
-      <c r="D24" s="86" t="s">
-        <v>182</v>
-      </c>
+      <c r="D24" s="86"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="85"/>
       <c r="B25" s="85"/>
-      <c r="D25" s="86" t="s">
-        <v>185</v>
-      </c>
+      <c r="D25" s="86"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="85"/>
       <c r="B26" s="85"/>
-      <c r="D26" s="86" t="s">
-        <v>188</v>
-      </c>
+      <c r="D26" s="86"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="85"/>
       <c r="B27" s="85"/>
-      <c r="D27" s="86" t="s">
-        <v>191</v>
-      </c>
+      <c r="D27" s="86"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="85"/>
       <c r="B28" s="85"/>
-      <c r="D28" s="86" t="s">
-        <v>194</v>
-      </c>
+      <c r="D28" s="86"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="85"/>
       <c r="B29" s="85"/>
-      <c r="D29" s="86" t="s">
-        <v>197</v>
-      </c>
+      <c r="D29" s="86"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="85"/>
       <c r="B30" s="85"/>
-      <c r="D30" s="86" t="s">
-        <v>200</v>
-      </c>
+      <c r="D30" s="86"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="85"/>
       <c r="B31" s="85"/>
-      <c r="D31" s="86" t="s">
-        <v>204</v>
-      </c>
+      <c r="D31" s="86"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="85"/>
       <c r="B32" s="85"/>
-      <c r="D32" s="86" t="s">
-        <v>207</v>
-      </c>
+      <c r="D32" s="86"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="85"/>
       <c r="B33" s="85"/>
-      <c r="D33" s="86" t="s">
-        <v>210</v>
-      </c>
+      <c r="D33" s="86"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="85"/>
       <c r="B34" s="85"/>
-      <c r="D34" s="86" t="s">
-        <v>213</v>
-      </c>
+      <c r="D34" s="86"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="85"/>
       <c r="B35" s="85"/>
-      <c r="D35" s="86" t="s">
-        <v>216</v>
-      </c>
+      <c r="D35" s="86"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="85"/>
       <c r="B36" s="85"/>
-      <c r="D36" s="86" t="s">
-        <v>219</v>
-      </c>
+      <c r="D36" s="86"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="85"/>
       <c r="B37" s="85"/>
-      <c r="D37" s="86" t="s">
-        <v>222</v>
-      </c>
+      <c r="D37" s="86"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="85"/>
       <c r="B38" s="85"/>
-      <c r="D38" s="86" t="s">
-        <v>225</v>
-      </c>
+      <c r="D38" s="86"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="85"/>
       <c r="B39" s="85"/>
-      <c r="D39" s="86" t="s">
-        <v>228</v>
-      </c>
+      <c r="D39" s="86"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="85"/>
       <c r="B40" s="85"/>
-      <c r="D40" s="86" t="s">
-        <v>231</v>
-      </c>
+      <c r="D40" s="86"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="85"/>
       <c r="B41" s="85"/>
-      <c r="D41" s="86" t="s">
-        <v>234</v>
-      </c>
+      <c r="D41" s="86"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="85"/>
       <c r="B42" s="85"/>
-      <c r="D42" s="86" t="s">
-        <v>237</v>
-      </c>
+      <c r="D42" s="86"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="85"/>
       <c r="B43" s="85"/>
-      <c r="D43" s="86" t="s">
-        <v>240</v>
-      </c>
+      <c r="D43" s="86"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="85"/>
       <c r="B44" s="85"/>
-      <c r="D44" s="86" t="s">
-        <v>243</v>
-      </c>
+      <c r="D44" s="86"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="85"/>
       <c r="B45" s="85"/>
-      <c r="D45" s="86" t="s">
-        <v>246</v>
-      </c>
+      <c r="D45" s="86"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="85"/>
       <c r="B46" s="85"/>
-      <c r="D46" s="86" t="s">
-        <v>249</v>
-      </c>
+      <c r="D46" s="86"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="85"/>
       <c r="B47" s="85"/>
-      <c r="D47" s="86" t="s">
-        <v>252</v>
-      </c>
+      <c r="D47" s="86"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="85"/>
       <c r="B48" s="85"/>
-      <c r="D48" s="86" t="s">
-        <v>255</v>
-      </c>
+      <c r="D48" s="86"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="85"/>
       <c r="B49" s="85"/>
-      <c r="D49" s="86" t="s">
-        <v>258</v>
-      </c>
+      <c r="D49" s="86"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="85"/>
       <c r="B50" s="85"/>
-      <c r="D50" s="86" t="s">
-        <v>261</v>
-      </c>
+      <c r="D50" s="86"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="85"/>
       <c r="B51" s="85"/>
-      <c r="D51" s="86" t="s">
-        <v>264</v>
-      </c>
+      <c r="D51" s="86"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="85"/>
       <c r="B52" s="85"/>
-      <c r="D52" s="86" t="s">
-        <v>267</v>
-      </c>
+      <c r="D52" s="86"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="85"/>
       <c r="B53" s="85"/>
-      <c r="D53" s="86" t="s">
-        <v>270</v>
-      </c>
+      <c r="D53" s="86"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="85"/>
       <c r="B54" s="85"/>
-      <c r="D54" s="86" t="s">
-        <v>273</v>
-      </c>
+      <c r="D54" s="86"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="85"/>
       <c r="B55" s="85"/>
-      <c r="D55" s="86" t="s">
-        <v>276</v>
-      </c>
+      <c r="D55" s="86"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="85"/>
       <c r="B56" s="85"/>
-      <c r="D56" s="86" t="s">
-        <v>280</v>
-      </c>
+      <c r="D56" s="86"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="85"/>
       <c r="B57" s="85"/>
-      <c r="D57" s="86" t="s">
-        <v>283</v>
-      </c>
+      <c r="D57" s="86"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="85"/>
       <c r="B58" s="85"/>
-      <c r="D58" s="86" t="s">
-        <v>286</v>
-      </c>
+      <c r="D58" s="86"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="85"/>
       <c r="B59" s="85"/>
-      <c r="D59" s="86" t="s">
-        <v>289</v>
-      </c>
+      <c r="D59" s="86"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="85"/>
       <c r="B60" s="85"/>
-      <c r="D60" s="86" t="s">
-        <v>292</v>
-      </c>
+      <c r="D60" s="86"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="85"/>
       <c r="B61" s="85"/>
-      <c r="D61" s="86" t="s">
-        <v>295</v>
-      </c>
+      <c r="D61" s="86"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="85"/>
       <c r="B62" s="85"/>
-      <c r="D62" s="86" t="s">
-        <v>298</v>
-      </c>
+      <c r="D62" s="86"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="85"/>
       <c r="B63" s="85"/>
-      <c r="D63" s="86" t="s">
-        <v>301</v>
-      </c>
+      <c r="D63" s="86"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="85"/>
       <c r="B64" s="85"/>
-      <c r="D64" s="86" t="s">
-        <v>304</v>
-      </c>
+      <c r="D64" s="86"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="85"/>
       <c r="B65" s="85"/>
-      <c r="D65" s="86" t="s">
-        <v>307</v>
-      </c>
+      <c r="D65" s="86"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="85"/>
       <c r="B66" s="85"/>
-      <c r="D66" s="86" t="s">
-        <v>310</v>
-      </c>
+      <c r="D66" s="86"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="85"/>
       <c r="B67" s="85"/>
-      <c r="D67" s="86" t="s">
-        <v>313</v>
-      </c>
+      <c r="D67" s="86"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="85"/>
       <c r="B68" s="85"/>
-      <c r="D68" s="86" t="s">
-        <v>317</v>
-      </c>
+      <c r="D68" s="86"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="85"/>
       <c r="B69" s="85"/>
-      <c r="D69" s="86" t="s">
-        <v>320</v>
-      </c>
+      <c r="D69" s="86"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="85"/>
       <c r="B70" s="85"/>
-      <c r="D70" s="86" t="s">
-        <v>323</v>
-      </c>
+      <c r="D70" s="86"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="85"/>
       <c r="B71" s="85"/>
-      <c r="D71" s="86" t="s">
-        <v>326</v>
-      </c>
+      <c r="D71" s="86"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="85"/>
       <c r="B72" s="85"/>
-      <c r="D72" s="86" t="s">
-        <v>329</v>
-      </c>
+      <c r="D72" s="86"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="85"/>
       <c r="B73" s="85"/>
-      <c r="D73" s="86" t="s">
-        <v>332</v>
-      </c>
+      <c r="D73" s="86"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="85"/>
       <c r="B74" s="85"/>
-      <c r="D74" s="86" t="s">
-        <v>335</v>
-      </c>
+      <c r="D74" s="86"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="85"/>
       <c r="B75" s="85"/>
-      <c r="D75" s="86" t="s">
-        <v>338</v>
-      </c>
+      <c r="D75" s="86"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="85"/>
       <c r="B76" s="85"/>
-      <c r="D76" s="86" t="s">
-        <v>341</v>
-      </c>
+      <c r="D76" s="86"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="85"/>
       <c r="B77" s="85"/>
-      <c r="D77" s="86" t="s">
-        <v>344</v>
-      </c>
+      <c r="D77" s="86"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="85"/>
       <c r="B78" s="85"/>
-      <c r="D78" s="86" t="s">
-        <v>347</v>
-      </c>
+      <c r="D78" s="86"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="85"/>
       <c r="B79" s="85"/>
-      <c r="D79" s="86" t="s">
-        <v>349</v>
-      </c>
+      <c r="D79" s="86"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="85"/>
       <c r="B80" s="85"/>
-      <c r="D80" s="86" t="s">
-        <v>352</v>
-      </c>
+      <c r="D80" s="86"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="85"/>
       <c r="B81" s="85"/>
-      <c r="D81" s="86" t="s">
-        <v>355</v>
-      </c>
+      <c r="D81" s="86"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="85"/>
       <c r="B82" s="85"/>
-      <c r="D82" s="86" t="s">
-        <v>358</v>
-      </c>
+      <c r="D82" s="86"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="85"/>
       <c r="B83" s="85"/>
-      <c r="D83" s="86" t="s">
-        <v>361</v>
-      </c>
+      <c r="D83" s="86"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="85"/>
       <c r="B84" s="85"/>
-      <c r="D84" s="86" t="s">
-        <v>364</v>
-      </c>
+      <c r="D84" s="86"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="85"/>
       <c r="B85" s="85"/>
-      <c r="D85" s="86" t="s">
-        <v>367</v>
-      </c>
+      <c r="D85" s="86"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="85"/>
       <c r="B86" s="85"/>
-      <c r="D86" s="86" t="s">
-        <v>370</v>
-      </c>
+      <c r="D86" s="86"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="85"/>
       <c r="B87" s="85"/>
-      <c r="D87" s="86" t="s">
-        <v>373</v>
-      </c>
+      <c r="D87" s="86"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="85"/>
       <c r="B88" s="85"/>
-      <c r="D88" s="86" t="s">
-        <v>376</v>
-      </c>
+      <c r="D88" s="86"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="85"/>
       <c r="B89" s="85"/>
-      <c r="D89" s="86" t="s">
-        <v>379</v>
-      </c>
+      <c r="D89" s="86"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="85"/>
       <c r="B90" s="85"/>
-      <c r="D90" s="86" t="s">
-        <v>382</v>
-      </c>
+      <c r="D90" s="86"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="85"/>
       <c r="B91" s="85"/>
-      <c r="D91" s="86" t="s">
-        <v>385</v>
-      </c>
+      <c r="D91" s="86"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="85"/>
       <c r="B92" s="85"/>
-      <c r="D92" s="86" t="s">
-        <v>388</v>
-      </c>
+      <c r="D92" s="86"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="85"/>
       <c r="B93" s="85"/>
-      <c r="D93" s="86" t="s">
-        <v>391</v>
-      </c>
+      <c r="D93" s="86"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="85"/>
       <c r="B94" s="85"/>
-      <c r="D94" s="86" t="s">
-        <v>394</v>
-      </c>
+      <c r="D94" s="86"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="85"/>
       <c r="B95" s="85"/>
-      <c r="D95" s="86" t="s">
-        <v>397</v>
-      </c>
+      <c r="D95" s="86"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="85"/>
       <c r="B96" s="85"/>
-      <c r="D96" s="86" t="s">
-        <v>399</v>
-      </c>
+      <c r="D96" s="86"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="85"/>
       <c r="B97" s="85"/>
-      <c r="D97" s="86" t="s">
-        <v>402</v>
-      </c>
+      <c r="D97" s="86"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="85"/>
       <c r="B98" s="85"/>
-      <c r="D98" s="86" t="s">
-        <v>405</v>
-      </c>
+      <c r="D98" s="86"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="85"/>
       <c r="B99" s="85"/>
-      <c r="D99" s="86" t="s">
-        <v>408</v>
-      </c>
+      <c r="D99" s="86"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="85"/>
       <c r="B100" s="85"/>
-      <c r="D100" s="86" t="s">
-        <v>410</v>
-      </c>
+      <c r="D100" s="86"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="85"/>
       <c r="B101" s="85"/>
-      <c r="D101" s="86" t="s">
-        <v>412</v>
-      </c>
+      <c r="D101" s="86"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="85"/>
       <c r="B102" s="85"/>
-      <c r="D102" s="86" t="s">
-        <v>414</v>
-      </c>
+      <c r="D102" s="86"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="85"/>
       <c r="B103" s="85"/>
-      <c r="D103" s="86" t="s">
-        <v>416</v>
-      </c>
+      <c r="D103" s="86"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="85"/>
       <c r="B104" s="85"/>
-      <c r="D104" s="86" t="s">
-        <v>418</v>
-      </c>
+      <c r="D104" s="86"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="85"/>
       <c r="B105" s="85"/>
-      <c r="D105" s="86" t="s">
-        <v>421</v>
-      </c>
+      <c r="D105" s="86"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="85"/>
       <c r="B106" s="85"/>
-      <c r="D106" s="86" t="s">
-        <v>424</v>
-      </c>
+      <c r="D106" s="86"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="85"/>
       <c r="B107" s="85"/>
-      <c r="D107" s="86" t="s">
-        <v>427</v>
-      </c>
+      <c r="D107" s="86"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="85"/>
       <c r="B108" s="85"/>
-      <c r="D108" s="86" t="s">
-        <v>430</v>
-      </c>
+      <c r="D108" s="86"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="85"/>
       <c r="B109" s="85"/>
-      <c r="D109" s="86" t="s">
-        <v>433</v>
-      </c>
+      <c r="D109" s="86"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="85"/>
       <c r="B110" s="85"/>
-      <c r="D110" s="86" t="s">
-        <v>437</v>
-      </c>
+      <c r="D110" s="86"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="85"/>
       <c r="B111" s="85"/>
-      <c r="D111" s="86" t="s">
-        <v>440</v>
-      </c>
+      <c r="D111" s="86"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="85"/>
       <c r="B112" s="85"/>
-      <c r="D112" s="86" t="s">
-        <v>443</v>
-      </c>
+      <c r="D112" s="86"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="85"/>
       <c r="B113" s="85"/>
-      <c r="D113" s="86" t="s">
-        <v>446</v>
-      </c>
+      <c r="D113" s="86"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="85"/>
       <c r="B114" s="85"/>
-      <c r="D114" s="86" t="s">
-        <v>449</v>
-      </c>
+      <c r="D114" s="86"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="85"/>
       <c r="B115" s="85"/>
-      <c r="D115" s="86" t="s">
-        <v>452</v>
-      </c>
+      <c r="D115" s="86"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="85"/>
       <c r="B116" s="85"/>
-      <c r="D116" s="86" t="s">
-        <v>455</v>
-      </c>
+      <c r="D116" s="86"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="85"/>
       <c r="B117" s="85"/>
-      <c r="D117" s="86" t="s">
-        <v>458</v>
-      </c>
+      <c r="D117" s="86"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="85"/>
       <c r="B118" s="85"/>
-      <c r="D118" s="86" t="s">
-        <v>461</v>
-      </c>
+      <c r="D118" s="86"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="85"/>
       <c r="B119" s="85"/>
-      <c r="D119" s="86" t="s">
-        <v>464</v>
-      </c>
+      <c r="D119" s="86"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="85"/>
       <c r="B120" s="85"/>
-      <c r="D120" s="86" t="s">
-        <v>467</v>
-      </c>
+      <c r="D120" s="86"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="85"/>
       <c r="B121" s="85"/>
-      <c r="D121" s="86" t="s">
-        <v>470</v>
-      </c>
+      <c r="D121" s="86"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="85"/>
       <c r="B122" s="85"/>
-      <c r="D122" s="86" t="s">
-        <v>473</v>
-      </c>
+      <c r="D122" s="86"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="85"/>
       <c r="B123" s="85"/>
-      <c r="D123" s="86" t="s">
-        <v>476</v>
-      </c>
+      <c r="D123" s="86"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="85"/>
       <c r="B124" s="85"/>
-      <c r="D124" s="86" t="s">
-        <v>479</v>
-      </c>
+      <c r="D124" s="86"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="85"/>
       <c r="B125" s="85"/>
-      <c r="D125" s="86" t="s">
-        <v>482</v>
-      </c>
+      <c r="D125" s="86"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="85"/>
       <c r="B126" s="85"/>
-      <c r="D126" s="86" t="s">
-        <v>485</v>
-      </c>
+      <c r="D126" s="86"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="85"/>
       <c r="B127" s="85"/>
-      <c r="D127" s="86" t="s">
-        <v>488</v>
-      </c>
+      <c r="D127" s="86"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="85"/>
       <c r="B128" s="85"/>
-      <c r="D128" s="86" t="s">
-        <v>491</v>
-      </c>
+      <c r="D128" s="86"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="85"/>
       <c r="B129" s="85"/>
-      <c r="D129" s="86" t="s">
-        <v>494</v>
-      </c>
+      <c r="D129" s="86"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="85"/>
       <c r="B130" s="85"/>
-      <c r="D130" s="86" t="s">
-        <v>497</v>
-      </c>
+      <c r="D130" s="86"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="85"/>
       <c r="B131" s="85"/>
-      <c r="D131" s="86" t="s">
-        <v>500</v>
-      </c>
+      <c r="D131" s="86"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="85"/>
       <c r="B132" s="85"/>
-      <c r="D132" s="86" t="s">
-        <v>503</v>
-      </c>
+      <c r="D132" s="86"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="85"/>
       <c r="B133" s="85"/>
-      <c r="D133" s="86" t="s">
-        <v>506</v>
-      </c>
+      <c r="D133" s="86"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="85"/>
       <c r="B134" s="85"/>
-      <c r="D134" s="86" t="s">
-        <v>509</v>
-      </c>
+      <c r="D134" s="86"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="85"/>
       <c r="B135" s="85"/>
-      <c r="D135" s="86" t="s">
-        <v>512</v>
-      </c>
+      <c r="D135" s="86"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="85"/>
       <c r="B136" s="85"/>
-      <c r="D136" s="86" t="s">
-        <v>515</v>
-      </c>
+      <c r="D136" s="86"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="85"/>
       <c r="B137" s="85"/>
-      <c r="D137" s="86" t="s">
-        <v>518</v>
-      </c>
+      <c r="D137" s="86"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="85"/>
       <c r="B138" s="85"/>
-      <c r="D138" s="86" t="s">
-        <v>521</v>
-      </c>
+      <c r="D138" s="86"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="85"/>
       <c r="B139" s="85"/>
-      <c r="D139" s="86" t="s">
-        <v>524</v>
-      </c>
+      <c r="D139" s="86"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="85"/>
       <c r="B140" s="85"/>
-      <c r="D140" s="86" t="s">
-        <v>524</v>
-      </c>
+      <c r="D140" s="86"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="85"/>
       <c r="B141" s="85"/>
-      <c r="D141" s="86" t="s">
-        <v>529</v>
-      </c>
+      <c r="D141" s="86"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="85"/>
       <c r="B142" s="85"/>
-      <c r="D142" s="86" t="s">
-        <v>532</v>
-      </c>
+      <c r="D142" s="86"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="85"/>
       <c r="B143" s="85"/>
-      <c r="D143" s="86" t="s">
-        <v>535</v>
-      </c>
+      <c r="D143" s="86"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="85"/>
       <c r="B144" s="85"/>
-      <c r="D144" s="86" t="s">
-        <v>538</v>
-      </c>
+      <c r="D144" s="86"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="85"/>
       <c r="B145" s="85"/>
-      <c r="D145" s="86" t="s">
-        <v>541</v>
-      </c>
+      <c r="D145" s="86"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="85"/>
       <c r="B146" s="85"/>
-      <c r="D146" s="86" t="s">
-        <v>544</v>
-      </c>
+      <c r="D146" s="86"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="85"/>
       <c r="B147" s="85"/>
-      <c r="D147" s="86" t="s">
-        <v>547</v>
-      </c>
+      <c r="D147" s="86"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="85"/>
       <c r="B148" s="85"/>
-      <c r="D148" s="86" t="s">
-        <v>547</v>
-      </c>
+      <c r="D148" s="86"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="85"/>
       <c r="B149" s="85"/>
-      <c r="D149" s="86" t="s">
-        <v>552</v>
-      </c>
+      <c r="D149" s="86"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="85"/>
       <c r="B150" s="85"/>
-      <c r="D150" s="86" t="s">
-        <v>555</v>
-      </c>
+      <c r="D150" s="86"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="85"/>
       <c r="B151" s="85"/>
-      <c r="D151" s="86" t="s">
-        <v>558</v>
-      </c>
+      <c r="D151" s="86"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="85"/>
       <c r="B152" s="85"/>
-      <c r="D152" s="86" t="s">
-        <v>561</v>
-      </c>
+      <c r="D152" s="86"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="85"/>
       <c r="B153" s="85"/>
-      <c r="D153" s="86" t="s">
-        <v>564</v>
-      </c>
+      <c r="D153" s="86"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="85"/>
       <c r="B154" s="85"/>
-      <c r="D154" s="86" t="s">
-        <v>567</v>
-      </c>
+      <c r="D154" s="86"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="85"/>
       <c r="B155" s="85"/>
-      <c r="D155" s="86" t="s">
-        <v>570</v>
-      </c>
+      <c r="D155" s="86"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="85"/>
       <c r="B156" s="85"/>
-      <c r="D156" s="86" t="s">
-        <v>573</v>
-      </c>
+      <c r="D156" s="86"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="85"/>
       <c r="B157" s="85"/>
-      <c r="D157" s="86" t="s">
-        <v>576</v>
-      </c>
+      <c r="D157" s="86"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="85"/>
       <c r="B158" s="85"/>
-      <c r="D158" s="86" t="s">
-        <v>579</v>
-      </c>
+      <c r="D158" s="86"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="85"/>
       <c r="B159" s="85"/>
-      <c r="D159" s="86" t="s">
-        <v>583</v>
-      </c>
+      <c r="D159" s="86"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="85"/>
       <c r="B160" s="85"/>
-      <c r="D160" s="86" t="s">
-        <v>586</v>
-      </c>
+      <c r="D160" s="86"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="85"/>
       <c r="B161" s="85"/>
-      <c r="D161" s="86" t="s">
-        <v>589</v>
-      </c>
+      <c r="D161" s="86"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="85"/>
       <c r="B162" s="85"/>
-      <c r="D162" s="86" t="s">
-        <v>592</v>
-      </c>
+      <c r="D162" s="86"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="85"/>
       <c r="B163" s="85"/>
-      <c r="D163" s="86" t="s">
-        <v>595</v>
-      </c>
+      <c r="D163" s="86"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="85"/>
       <c r="B164" s="85"/>
-      <c r="D164" s="86" t="s">
-        <v>595</v>
-      </c>
+      <c r="D164" s="86"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="85"/>
       <c r="B165" s="85"/>
-      <c r="D165" s="86" t="s">
-        <v>600</v>
-      </c>
+      <c r="D165" s="86"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="85"/>
       <c r="B166" s="85"/>
-      <c r="D166" s="86" t="s">
-        <v>603</v>
-      </c>
+      <c r="D166" s="86"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="85"/>
       <c r="B167" s="85"/>
-      <c r="D167" s="86" t="s">
-        <v>606</v>
-      </c>
+      <c r="D167" s="86"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="85"/>
       <c r="B168" s="85"/>
-      <c r="D168" s="86" t="s">
-        <v>609</v>
-      </c>
+      <c r="D168" s="86"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="85"/>
       <c r="B169" s="85"/>
-      <c r="D169" s="86" t="s">
-        <v>612</v>
-      </c>
+      <c r="D169" s="86"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="85"/>
       <c r="B170" s="85"/>
-      <c r="D170" s="86" t="s">
-        <v>615</v>
-      </c>
+      <c r="D170" s="86"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="85"/>
       <c r="B171" s="85"/>
-      <c r="D171" s="86" t="s">
-        <v>618</v>
-      </c>
+      <c r="D171" s="86"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="85"/>
       <c r="B172" s="85"/>
-      <c r="D172" s="86" t="s">
-        <v>621</v>
-      </c>
+      <c r="D172" s="86"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="85"/>
       <c r="B173" s="85"/>
-      <c r="D173" s="86" t="s">
-        <v>624</v>
-      </c>
+      <c r="D173" s="86"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="85"/>
       <c r="B174" s="85"/>
-      <c r="D174" s="86" t="s">
-        <v>627</v>
-      </c>
+      <c r="D174" s="86"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="85"/>
       <c r="B175" s="85"/>
-      <c r="D175" s="86" t="s">
-        <v>630</v>
-      </c>
+      <c r="D175" s="86"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="85"/>
       <c r="B176" s="85"/>
-      <c r="D176" s="86" t="s">
-        <v>633</v>
-      </c>
+      <c r="D176" s="86"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="85"/>
       <c r="B177" s="85"/>
-      <c r="D177" s="86" t="s">
-        <v>636</v>
-      </c>
+      <c r="D177" s="86"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="85"/>
       <c r="B178" s="85"/>
-      <c r="D178" s="86" t="s">
-        <v>639</v>
-      </c>
+      <c r="D178" s="86"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="85"/>
       <c r="B179" s="85"/>
-      <c r="D179" s="86" t="s">
-        <v>642</v>
-      </c>
+      <c r="D179" s="86"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="85"/>
       <c r="B180" s="85"/>
-      <c r="D180" s="86" t="s">
-        <v>645</v>
-      </c>
+      <c r="D180" s="86"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="85"/>
       <c r="B181" s="85"/>
-      <c r="D181" s="86" t="s">
-        <v>648</v>
-      </c>
+      <c r="D181" s="86"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="85"/>
       <c r="B182" s="85"/>
-      <c r="D182" s="86" t="s">
-        <v>651</v>
-      </c>
+      <c r="D182" s="86"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="85"/>
       <c r="B183" s="85"/>
-      <c r="D183" s="86" t="s">
-        <v>654</v>
-      </c>
+      <c r="D183" s="86"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="85"/>
       <c r="B184" s="85"/>
-      <c r="D184" s="86" t="s">
-        <v>657</v>
-      </c>
+      <c r="D184" s="86"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="85"/>
       <c r="B185" s="85"/>
-      <c r="D185" s="86" t="s">
-        <v>660</v>
-      </c>
+      <c r="D185" s="86"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="85"/>
       <c r="B186" s="85"/>
-      <c r="D186" s="86" t="s">
-        <v>663</v>
-      </c>
+      <c r="D186" s="86"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="85"/>
       <c r="B187" s="85"/>
-      <c r="D187" s="86" t="s">
-        <v>666</v>
-      </c>
+      <c r="D187" s="86"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="85"/>
       <c r="B188" s="85"/>
-      <c r="D188" s="86" t="s">
-        <v>669</v>
-      </c>
+      <c r="D188" s="86"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="85"/>
       <c r="B189" s="85"/>
-      <c r="D189" s="86" t="s">
-        <v>672</v>
-      </c>
+      <c r="D189" s="86"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="85"/>
       <c r="B190" s="85"/>
-      <c r="D190" s="86" t="s">
-        <v>675</v>
-      </c>
+      <c r="D190" s="86"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="85"/>
       <c r="B191" s="85"/>
-      <c r="D191" s="86" t="s">
-        <v>678</v>
-      </c>
+      <c r="D191" s="86"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="85"/>
       <c r="B192" s="85"/>
-      <c r="D192" s="86" t="s">
-        <v>470</v>
-      </c>
+      <c r="D192" s="86"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="85"/>
       <c r="B193" s="85"/>
-      <c r="D193" s="86" t="s">
-        <v>683</v>
-      </c>
+      <c r="D193" s="86"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="85"/>
       <c r="B194" s="85"/>
-      <c r="D194" s="86" t="s">
-        <v>686</v>
-      </c>
+      <c r="D194" s="86"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="85"/>
       <c r="B195" s="85"/>
-      <c r="D195" s="86" t="s">
-        <v>689</v>
-      </c>
+      <c r="D195" s="86"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="85"/>
       <c r="B196" s="85"/>
-      <c r="D196" s="86" t="s">
-        <v>692</v>
-      </c>
+      <c r="D196" s="86"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="85"/>
       <c r="B197" s="85"/>
-      <c r="D197" s="86" t="s">
-        <v>695</v>
-      </c>
+      <c r="D197" s="86"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="85"/>
       <c r="B198" s="85"/>
-      <c r="D198" s="86" t="s">
-        <v>698</v>
-      </c>
+      <c r="D198" s="86"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="85"/>
       <c r="B199" s="85"/>
-      <c r="D199" s="86" t="s">
-        <v>701</v>
-      </c>
+      <c r="D199" s="86"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="85"/>
       <c r="B200" s="85"/>
-      <c r="D200" s="86" t="s">
-        <v>704</v>
-      </c>
+      <c r="D200" s="86"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="85"/>
       <c r="B201" s="85"/>
-      <c r="D201" s="86" t="s">
-        <v>707</v>
-      </c>
+      <c r="D201" s="86"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="85"/>
       <c r="B202" s="85"/>
-      <c r="D202" s="86" t="s">
-        <v>710</v>
-      </c>
+      <c r="D202" s="86"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="85"/>
       <c r="B203" s="85"/>
-      <c r="D203" s="86" t="s">
-        <v>713</v>
-      </c>
+      <c r="D203" s="86"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="85"/>
       <c r="B204" s="85"/>
-      <c r="D204" s="86" t="s">
-        <v>716</v>
-      </c>
+      <c r="D204" s="86"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="85"/>
       <c r="B205" s="85"/>
-      <c r="D205" s="86" t="s">
-        <v>719</v>
-      </c>
+      <c r="D205" s="86"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="85"/>
       <c r="B206" s="85"/>
-      <c r="D206" s="86" t="s">
-        <v>722</v>
-      </c>
+      <c r="D206" s="86"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="85"/>
       <c r="B207" s="85"/>
-      <c r="D207" s="86" t="s">
-        <v>725</v>
-      </c>
+      <c r="D207" s="86"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="85"/>
       <c r="B208" s="85"/>
-      <c r="D208" s="86" t="s">
-        <v>728</v>
-      </c>
+      <c r="D208" s="86"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="85"/>
       <c r="B209" s="85"/>
-      <c r="D209" s="86" t="s">
-        <v>731</v>
-      </c>
+      <c r="D209" s="86"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="85"/>
       <c r="B210" s="85"/>
-      <c r="D210" s="86" t="s">
-        <v>734</v>
-      </c>
+      <c r="D210" s="86"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="85"/>
       <c r="B211" s="85"/>
-      <c r="D211" s="86" t="s">
-        <v>737</v>
-      </c>
+      <c r="D211" s="86"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="85"/>
       <c r="B212" s="85"/>
-      <c r="D212" s="86" t="s">
-        <v>740</v>
-      </c>
+      <c r="D212" s="86"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="85"/>
       <c r="B213" s="85"/>
-      <c r="D213" s="86" t="s">
-        <v>743</v>
-      </c>
+      <c r="D213" s="86"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="85"/>
       <c r="B214" s="85"/>
-      <c r="D214" s="86" t="s">
-        <v>746</v>
-      </c>
+      <c r="D214" s="86"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="85"/>
       <c r="B215" s="85"/>
-      <c r="D215" s="86" t="s">
-        <v>749</v>
-      </c>
+      <c r="D215" s="86"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="85"/>
       <c r="B216" s="85"/>
-      <c r="D216" s="86" t="s">
-        <v>752</v>
-      </c>
+      <c r="D216" s="86"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="85"/>
       <c r="B217" s="85"/>
-      <c r="D217" s="86" t="s">
-        <v>755</v>
-      </c>
+      <c r="D217" s="86"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="85"/>
       <c r="B218" s="85"/>
-      <c r="D218" s="86" t="s">
-        <v>758</v>
-      </c>
+      <c r="D218" s="86"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="85"/>
       <c r="B219" s="85"/>
-      <c r="D219" s="86" t="s">
-        <v>761</v>
-      </c>
+      <c r="D219" s="86"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="85"/>
       <c r="B220" s="85"/>
-      <c r="D220" s="86" t="s">
-        <v>764</v>
-      </c>
+      <c r="D220" s="86"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="85"/>
       <c r="B221" s="85"/>
-      <c r="D221" s="86" t="s">
-        <v>767</v>
-      </c>
+      <c r="D221" s="86"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="85"/>
       <c r="B222" s="85"/>
-      <c r="D222" s="86" t="s">
-        <v>770</v>
-      </c>
+      <c r="D222" s="86"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="85"/>
       <c r="B223" s="85"/>
-      <c r="D223" s="86" t="s">
-        <v>773</v>
-      </c>
+      <c r="D223" s="86"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="85"/>
       <c r="B224" s="85"/>
-      <c r="D224" s="86" t="s">
-        <v>776</v>
-      </c>
+      <c r="D224" s="86"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="85"/>
       <c r="B225" s="85"/>
-      <c r="D225" s="86" t="s">
-        <v>779</v>
-      </c>
+      <c r="D225" s="86"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="85"/>
       <c r="B226" s="85"/>
-      <c r="D226" s="86" t="s">
-        <v>783</v>
-      </c>
+      <c r="D226" s="86"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="85"/>
       <c r="B227" s="85"/>
-      <c r="D227" s="86" t="s">
-        <v>786</v>
-      </c>
+      <c r="D227" s="86"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="85"/>
       <c r="B228" s="85"/>
-      <c r="D228" s="86" t="s">
-        <v>430</v>
-      </c>
+      <c r="D228" s="86"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="85"/>
       <c r="B229" s="85"/>
-      <c r="D229" s="86" t="s">
-        <v>791</v>
-      </c>
+      <c r="D229" s="86"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="85"/>
       <c r="B230" s="85"/>
-      <c r="D230" s="86" t="s">
-        <v>794</v>
-      </c>
+      <c r="D230" s="86"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="85"/>
       <c r="B231" s="85"/>
-      <c r="D231" s="86" t="s">
-        <v>797</v>
-      </c>
+      <c r="D231" s="86"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="85"/>
       <c r="B232" s="85"/>
-      <c r="D232" s="86" t="s">
-        <v>800</v>
-      </c>
+      <c r="D232" s="86"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="85"/>
       <c r="B233" s="85"/>
-      <c r="D233" s="86" t="s">
-        <v>803</v>
-      </c>
+      <c r="D233" s="86"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="85"/>
       <c r="B234" s="85"/>
-      <c r="D234" s="86" t="s">
-        <v>806</v>
-      </c>
+      <c r="D234" s="86"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="85"/>
       <c r="B235" s="85"/>
-      <c r="D235" s="86" t="s">
-        <v>809</v>
-      </c>
+      <c r="D235" s="86"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="85"/>
       <c r="B236" s="85"/>
-      <c r="D236" s="86" t="s">
-        <v>812</v>
-      </c>
+      <c r="D236" s="86"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="85"/>
       <c r="B237" s="85"/>
-      <c r="D237" s="86" t="s">
-        <v>815</v>
-      </c>
+      <c r="D237" s="86"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="85"/>
       <c r="B238" s="85"/>
-      <c r="D238" s="86" t="s">
-        <v>818</v>
-      </c>
+      <c r="D238" s="86"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="85"/>
       <c r="B239" s="85"/>
-      <c r="D239" s="86" t="s">
-        <v>820</v>
-      </c>
+      <c r="D239" s="86"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="85"/>
       <c r="B240" s="85"/>
-      <c r="D240" s="86" t="s">
-        <v>823</v>
-      </c>
+      <c r="D240" s="86"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="85"/>
       <c r="B241" s="85"/>
-      <c r="D241" s="86" t="s">
-        <v>827</v>
-      </c>
+      <c r="D241" s="86"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="85"/>
       <c r="B242" s="85"/>
-      <c r="D242" s="86" t="s">
-        <v>830</v>
-      </c>
+      <c r="D242" s="86"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="85"/>
       <c r="B243" s="85"/>
-      <c r="D243" s="86" t="s">
-        <v>834</v>
-      </c>
+      <c r="D243" s="86"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="85"/>
       <c r="B244" s="85"/>
-      <c r="D244" s="86" t="s">
-        <v>837</v>
-      </c>
+      <c r="D244" s="86"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="85"/>
       <c r="B245" s="85"/>
-      <c r="D245" s="86" t="s">
-        <v>840</v>
-      </c>
+      <c r="D245" s="86"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="85"/>
       <c r="B246" s="85"/>
-      <c r="D246" s="86" t="s">
-        <v>843</v>
-      </c>
+      <c r="D246" s="86"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="85"/>
       <c r="B247" s="85"/>
-      <c r="D247" s="86" t="s">
-        <v>846</v>
-      </c>
+      <c r="D247" s="86"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="85"/>
       <c r="B248" s="85"/>
-      <c r="D248" s="86" t="s">
-        <v>849</v>
-      </c>
+      <c r="D248" s="86"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="85"/>
       <c r="B249" s="85"/>
-      <c r="D249" s="86" t="s">
-        <v>852</v>
-      </c>
+      <c r="D249" s="86"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="85"/>
       <c r="B250" s="85"/>
-      <c r="D250" s="86" t="s">
-        <v>855</v>
-      </c>
+      <c r="D250" s="86"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="85"/>
       <c r="B251" s="85"/>
-      <c r="D251" s="86" t="s">
-        <v>858</v>
-      </c>
+      <c r="D251" s="86"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="85"/>
       <c r="B252" s="85"/>
-      <c r="D252" s="86" t="s">
-        <v>861</v>
-      </c>
+      <c r="D252" s="86"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="85"/>
       <c r="B253" s="85"/>
-      <c r="D253" s="86" t="s">
-        <v>864</v>
-      </c>
+      <c r="D253" s="86"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="85"/>
       <c r="B254" s="85"/>
-      <c r="D254" s="86" t="s">
-        <v>867</v>
-      </c>
+      <c r="D254" s="86"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="85"/>
       <c r="B255" s="85"/>
-      <c r="D255" s="86" t="s">
-        <v>870</v>
-      </c>
+      <c r="D255" s="86"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="85"/>
       <c r="B256" s="85"/>
-      <c r="D256" s="86" t="s">
-        <v>873</v>
-      </c>
+      <c r="D256" s="86"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="85"/>
       <c r="B257" s="85"/>
-      <c r="D257" s="86" t="s">
-        <v>876</v>
-      </c>
+      <c r="D257" s="86"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="85"/>
       <c r="B258" s="85"/>
-      <c r="D258" s="86" t="s">
-        <v>879</v>
-      </c>
+      <c r="D258" s="86"/>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="85"/>
       <c r="B259" s="85"/>
-      <c r="D259" s="86" t="s">
-        <v>882</v>
-      </c>
+      <c r="D259" s="86"/>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="85"/>
       <c r="B260" s="85"/>
-      <c r="D260" s="86" t="s">
-        <v>885</v>
-      </c>
+      <c r="D260" s="86"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="85"/>
       <c r="B261" s="85"/>
-      <c r="D261" s="86" t="s">
-        <v>888</v>
-      </c>
+      <c r="D261" s="86"/>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="85"/>
       <c r="B262" s="85"/>
-      <c r="D262" s="86" t="s">
-        <v>891</v>
-      </c>
+      <c r="D262" s="86"/>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="85"/>
       <c r="B263" s="85"/>
-      <c r="D263" s="86" t="s">
-        <v>894</v>
-      </c>
+      <c r="D263" s="86"/>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="85"/>
       <c r="B264" s="85"/>
-      <c r="D264" s="86" t="s">
-        <v>897</v>
-      </c>
+      <c r="D264" s="86"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="85"/>
       <c r="B265" s="85"/>
-      <c r="D265" s="86" t="s">
-        <v>900</v>
-      </c>
+      <c r="D265" s="86"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="85"/>
       <c r="B266" s="85"/>
-      <c r="D266" s="86" t="s">
-        <v>903</v>
-      </c>
+      <c r="D266" s="86"/>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="85"/>
       <c r="B267" s="85"/>
-      <c r="D267" s="86" t="s">
-        <v>906</v>
-      </c>
+      <c r="D267" s="86"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="85"/>
       <c r="B268" s="85"/>
-      <c r="D268" s="86" t="s">
-        <v>909</v>
-      </c>
+      <c r="D268" s="86"/>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="85"/>
       <c r="B269" s="85"/>
-      <c r="D269" s="86" t="s">
-        <v>912</v>
-      </c>
+      <c r="D269" s="86"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="85"/>
       <c r="B270" s="85"/>
-      <c r="D270" s="86" t="s">
-        <v>915</v>
-      </c>
+      <c r="D270" s="86"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="85"/>
       <c r="B271" s="85"/>
-      <c r="D271" s="86" t="s">
-        <v>918</v>
-      </c>
+      <c r="D271" s="86"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="85"/>
       <c r="B272" s="85"/>
-      <c r="D272" s="86" t="s">
-        <v>921</v>
-      </c>
+      <c r="D272" s="86"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="85"/>
       <c r="B273" s="85"/>
-      <c r="D273" s="86" t="s">
-        <v>924</v>
-      </c>
+      <c r="D273" s="86"/>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="85"/>
       <c r="B274" s="85"/>
-      <c r="D274" s="86" t="s">
-        <v>927</v>
-      </c>
+      <c r="D274" s="86"/>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="85"/>
       <c r="B275" s="85"/>
-      <c r="D275" s="86" t="s">
-        <v>930</v>
-      </c>
+      <c r="D275" s="86"/>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="85"/>
       <c r="B276" s="85"/>
-      <c r="D276" s="86" t="s">
-        <v>933</v>
-      </c>
+      <c r="D276" s="86"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="85"/>
       <c r="B277" s="85"/>
-      <c r="D277" s="86" t="s">
-        <v>936</v>
-      </c>
+      <c r="D277" s="86"/>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="85"/>
       <c r="B278" s="85"/>
-      <c r="D278" s="86" t="s">
-        <v>939</v>
-      </c>
+      <c r="D278" s="86"/>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="85"/>
       <c r="B279" s="85"/>
-      <c r="D279" s="86" t="s">
-        <v>942</v>
-      </c>
+      <c r="D279" s="86"/>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="85"/>
       <c r="B280" s="85"/>
-      <c r="D280" s="86" t="s">
-        <v>945</v>
-      </c>
+      <c r="D280" s="86"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="85"/>
       <c r="B281" s="85"/>
-      <c r="D281" s="86" t="s">
-        <v>948</v>
-      </c>
+      <c r="D281" s="86"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="85"/>
       <c r="B282" s="85"/>
-      <c r="D282" s="86" t="s">
-        <v>951</v>
-      </c>
+      <c r="D282" s="86"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="85"/>
       <c r="B283" s="85"/>
-      <c r="D283" s="86" t="s">
-        <v>954</v>
-      </c>
+      <c r="D283" s="86"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="85"/>
       <c r="B284" s="85"/>
-      <c r="D284" s="86" t="s">
-        <v>958</v>
-      </c>
+      <c r="D284" s="86"/>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="85"/>
       <c r="B285" s="85"/>
-      <c r="D285" s="86" t="s">
-        <v>961</v>
-      </c>
+      <c r="D285" s="86"/>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="85"/>
       <c r="B286" s="85"/>
-      <c r="D286" s="86" t="s">
-        <v>964</v>
-      </c>
+      <c r="D286" s="86"/>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="85"/>
       <c r="B287" s="85"/>
-      <c r="D287" s="86" t="s">
-        <v>967</v>
-      </c>
+      <c r="D287" s="86"/>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="85"/>
       <c r="B288" s="85"/>
-      <c r="D288" s="86" t="s">
-        <v>970</v>
-      </c>
+      <c r="D288" s="86"/>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="85"/>
       <c r="B289" s="85"/>
-      <c r="D289" s="86" t="s">
-        <v>249</v>
-      </c>
+      <c r="D289" s="86"/>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="85"/>
       <c r="B290" s="85"/>
-      <c r="D290" s="86" t="s">
-        <v>975</v>
-      </c>
+      <c r="D290" s="86"/>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="85"/>
       <c r="B291" s="85"/>
-      <c r="D291" s="86" t="s">
-        <v>978</v>
-      </c>
+      <c r="D291" s="86"/>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="85"/>
       <c r="B292" s="85"/>
-      <c r="D292" s="86" t="s">
-        <v>576</v>
-      </c>
+      <c r="D292" s="86"/>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="85"/>
       <c r="B293" s="85"/>
-      <c r="D293" s="86" t="s">
-        <v>983</v>
-      </c>
+      <c r="D293" s="86"/>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="85"/>
       <c r="B294" s="85"/>
-      <c r="D294" s="86" t="s">
-        <v>986</v>
-      </c>
+      <c r="D294" s="86"/>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="85"/>
       <c r="B295" s="85"/>
-      <c r="D295" s="86" t="s">
-        <v>989</v>
-      </c>
+      <c r="D295" s="86"/>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="85"/>
       <c r="B296" s="85"/>
-      <c r="D296" s="86" t="s">
-        <v>992</v>
-      </c>
+      <c r="D296" s="86"/>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="85"/>
       <c r="B297" s="85"/>
-      <c r="D297" s="86" t="s">
-        <v>995</v>
-      </c>
+      <c r="D297" s="86"/>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" s="85"/>
       <c r="B298" s="85"/>
-      <c r="D298" s="86" t="s">
-        <v>998</v>
-      </c>
+      <c r="D298" s="86"/>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" s="85"/>
       <c r="B299" s="85"/>
-      <c r="D299" s="86" t="s">
-        <v>1001</v>
-      </c>
+      <c r="D299" s="86"/>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" s="85"/>
       <c r="B300" s="85"/>
-      <c r="D300" s="86" t="s">
-        <v>1004</v>
-      </c>
+      <c r="D300" s="86"/>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" s="85"/>
       <c r="B301" s="85"/>
-      <c r="D301" s="86" t="s">
-        <v>1006</v>
-      </c>
+      <c r="D301" s="86"/>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" s="85"/>
       <c r="B302" s="85"/>
-      <c r="D302" s="86" t="s">
-        <v>1009</v>
-      </c>
+      <c r="D302" s="86"/>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" s="85"/>
       <c r="B303" s="85"/>
-      <c r="D303" s="86" t="s">
-        <v>1012</v>
-      </c>
+      <c r="D303" s="86"/>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" s="85"/>

</xml_diff>